<commit_message>
dataset template submission.xlsx normalized header
changed to match dataset description column headers
Submission Item -> Metadata element
Definition -> Description
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/submission.xlsx
+++ b/resources/DatasetTemplate/submission.xlsx
@@ -32,10 +32,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Submission Item</t>
-  </si>
-  <si>
-    <t>Definition</t>
+    <t>Metadata element</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>Value</t>

</xml_diff>

<commit_message>
DatasetTemplate updated to version 1.1
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/submission.xlsx
+++ b/resources/DatasetTemplate/submission.xlsx
@@ -32,10 +32,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Metadata element</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Submission Item</t>
+  </si>
+  <si>
+    <t>Definition</t>
   </si>
   <si>
     <t>Value</t>

</xml_diff>

<commit_message>
template submission file updated with instructions for external submissions
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/submission.xlsx
+++ b/resources/DatasetTemplate/submission.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,10 +31,40 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPARC Award number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grant number supporting the milestone</t>
+    <t xml:space="preserve">SPARC award number</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Grant number supporting the milestone. Use </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EXTERNAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> if dataset is not from SPARC.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Milestone achieved</t>
@@ -56,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -81,24 +111,17 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="13.95"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13.95"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="-webkit-standard"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -157,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,24 +189,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -259,66 +274,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" customFormat="false" ht="35.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" customFormat="false" ht="18.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="100" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" customFormat="false" ht="86.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>